<commit_message>
graph for report update
</commit_message>
<xml_diff>
--- a/Training_log.xlsx
+++ b/Training_log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halli\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://queensuca-my.sharepoint.com/personal/17bsh3_queensu_ca/Documents/Winter 2024/HPCP/Final Project/inverted_flywheel_pendulum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12B5507-87B9-4DA3-8A04-259EFFEE7470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{A12B5507-87B9-4DA3-8A04-259EFFEE7470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42DA06E8-040C-4782-A194-D51E346F31A2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>Trial</t>
+  </si>
+  <si>
+    <t>April 21 2024</t>
+  </si>
+  <si>
+    <t>not saved</t>
+  </si>
+  <si>
+    <t>Time [s]</t>
   </si>
 </sst>
 </file>
@@ -412,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -428,7 +437,7 @@
     <col min="9" max="9" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -462,8 +471,11 @@
       <c r="K1" t="s">
         <v>16</v>
       </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -498,12 +510,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -538,7 +550,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -571,6 +583,44 @@
       </c>
       <c r="K5" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>0.215</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>418.9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6">
+        <v>100</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6">
+        <v>1035.9739999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>